<commit_message>
added re-run and doc changes
</commit_message>
<xml_diff>
--- a/data/reference/what_is_blocked.xlsx
+++ b/data/reference/what_is_blocked.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>additional_info_link</t>
+          <t>background_info_link</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">lgbtq </t>
+          <t>lgbtq+</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">

</xml_diff>

<commit_message>
made tables for social justice
</commit_message>
<xml_diff>
--- a/data/reference/what_is_blocked.xlsx
+++ b/data/reference/what_is_blocked.xlsx
@@ -2017,7 +2017,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>american nazi party</t>
+          <t>dual seedline</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2027,23 +2027,27 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+      <c r="F61" t="n">
+        <v>31</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://www.splcenter.org/fighting-hate/intelligence-report/2015/active-neo-nazi-groups</t>
+          <t>https://www.adl.org/resources/backgrounders/christian-identity</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>aryan nation</t>
+          <t>globalist jews</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2053,27 +2057,27 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://www.adl.org/education/resources/profiles/aryan-nations</t>
+          <t>https://www.haaretz.com/us-news/.premium-how-did-the-term-globalist-became-an-anti-semitic-slur-blame-bannon-1.5895925</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>dindu</t>
+          <t>heil hitler</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2081,21 +2085,29 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>32571</v>
+      </c>
+      <c r="G63" t="n">
+        <v>3</v>
+      </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://www.vice.com/en/article/ezagwm/get-to-know-the-memes-of-the-alt-right-and-never-miss-a-dog-whistle-again</t>
+          <t>https://www.adl.org/education/references/hate-symbols/hitler-salute-hand-sign</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>dual seedline</t>
+          <t>jewish question</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2111,21 +2123,21 @@
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="n">
-        <v>31</v>
+        <v>10375</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://www.adl.org/resources/backgrounders/christian-identity</t>
+          <t>https://encyclopedia.ushmm.org/content/en/article/the-jewish-question</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>gas the kikes</t>
+          <t>radical islamic terror</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2135,27 +2147,27 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>1746</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>https://www.thedailybeast.com/youtube-wont-ban-neo-nazi-group-chanting-gas-the-kkes-race-war-now</t>
+          <t>http://csps.gmu.edu/2020/12/01/why-does-the-west-remain-so-obsessed-with-radical-islam/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>gas the kikes race war now</t>
+          <t>sieg heil</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2165,27 +2177,27 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Empty</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>32586</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>https://psmag.com/ideas/neo-nazi-hate-speech-foiling-algorithms</t>
+          <t>https://www.adl.org/education/references/hate-symbols/sieg-heil</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>globalist jews</t>
+          <t>white genocide</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2201,21 +2213,21 @@
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="n">
-        <v>6</v>
+        <v>22245</v>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>https://www.haaretz.com/us-news/.premium-how-did-the-term-globalist-became-an-anti-semitic-slur-blame-bannon-1.5895925</t>
+          <t>https://www.adl.org/resources/glossary-terms/white-genocide</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>goy</t>
+          <t>white nationalist</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2223,21 +2235,29 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>59520</v>
+      </c>
+      <c r="G68" t="n">
+        <v>13</v>
+      </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://www.adl.org/education/references/hate-symbols/the-goyim-knowshut-it-down</t>
+          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/white-nationalist</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>heil hitler</t>
+          <t>white pill</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2253,21 +2273,21 @@
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="n">
-        <v>32571</v>
+        <v>9423</v>
       </c>
       <c r="G69" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>https://www.adl.org/education/references/hate-symbols/hitler-salute-hand-sign</t>
+          <t>https://www.adl.org/blog/the-extremist-medicine-cabinet-a-guide-to-online-pills</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>holocaust denial</t>
+          <t>white pride</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2277,23 +2297,27 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
+      <c r="F70" t="n">
+        <v>19044</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1</v>
+      </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/holocaust-denial</t>
+          <t>https://www.adl.org/resources/glossary-terms/white-pride</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>holohoax</t>
+          <t>gas the kikes race war now</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2301,21 +2325,29 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Empty</t>
+        </is>
+      </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>https://www.isdglobal.org/isd-publications/hosting-the-holohoax-a-snapshot-of-holocaust-denial-across-social-media/</t>
+          <t>https://psmag.com/ideas/neo-nazi-hate-speech-foiling-algorithms</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>jewish question</t>
+          <t>aryan nation</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2325,27 +2357,27 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Partial Block</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="n">
-        <v>10375</v>
+        <v>1</v>
       </c>
       <c r="G72" t="n">
         <v>2</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>https://encyclopedia.ushmm.org/content/en/article/the-jewish-question</t>
+          <t>https://www.adl.org/education/resources/profiles/aryan-nations</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>kike</t>
+          <t>gas the kikes</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2353,21 +2385,29 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Partial Block</t>
+        </is>
+      </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
+      <c r="F73" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>https://blog.oup.com/2009/10/ethnic-slurs-kike/</t>
+          <t>https://www.thedailybeast.com/youtube-wont-ban-neo-nazi-group-chanting-gas-the-kkes-race-war-now</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>kkk</t>
+          <t>two seedline</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2375,21 +2415,29 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr"/>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Partial Block</t>
+        </is>
+      </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr"/>
+      <c r="F74" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/ku-klux-klan</t>
+          <t>https://www.splcenter.org/fighting-hate/intelligence-report/2008/branson-televangelist-arnold-murray-preaches-christian-identity-theology</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>nazi</t>
+          <t>american nazi party</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2397,21 +2445,25 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr">
         <is>
-          <t>https://www.adl.org/resources/glossary-terms/neo-nazis</t>
+          <t>https://www.splcenter.org/fighting-hate/intelligence-report/2015/active-neo-nazi-groups</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>neo-confederate</t>
+          <t>holocaust denial</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2419,21 +2471,25 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr">
         <is>
-          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/neo-confederate</t>
+          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/holocaust-denial</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>neo-nazi</t>
+          <t>white pride worldwide</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2441,21 +2497,25 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr">
         <is>
-          <t>https://www.adl.org/resources/glossary-terms/neo-nazis</t>
+          <t>https://www.splcenter.org/fighting-hate/extremist-files/group/stormfront</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>dindu</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2470,14 +2530,14 @@
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr">
         <is>
-          <t>https://www.washingtonpost.com/wp-srv/style/longterm/books/chap1/nigger.htm</t>
+          <t>https://www.vice.com/en/article/ezagwm/get-to-know-the-memes-of-the-alt-right-and-never-miss-a-dog-whistle-again</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>radical islamic terror</t>
+          <t>goy</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2485,29 +2545,21 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr"/>
-      <c r="F79" t="n">
-        <v>1746</v>
-      </c>
-      <c r="G79" t="n">
-        <v>0</v>
-      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr">
         <is>
-          <t>http://csps.gmu.edu/2020/12/01/why-does-the-west-remain-so-obsessed-with-radical-islam/</t>
+          <t>https://www.adl.org/education/references/hate-symbols/the-goyim-knowshut-it-down</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>sieg heil</t>
+          <t>holohoax</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2515,29 +2567,21 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
-      <c r="F80" t="n">
-        <v>32586</v>
-      </c>
-      <c r="G80" t="n">
-        <v>4</v>
-      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr">
         <is>
-          <t>https://www.adl.org/education/references/hate-symbols/sieg-heil</t>
+          <t>https://www.isdglobal.org/isd-publications/hosting-the-holohoax-a-snapshot-of-holocaust-denial-across-social-media/</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>stormfront</t>
+          <t>kike</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2552,14 +2596,14 @@
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
         <is>
-          <t>https://www.adl.org/education/references/hate-symbols/stormfront</t>
+          <t>https://blog.oup.com/2009/10/ethnic-slurs-kike/</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>two seedline</t>
+          <t>kkk</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2567,29 +2611,21 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Partial Block</t>
-        </is>
-      </c>
+      <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
-      <c r="F82" t="n">
-        <v>1</v>
-      </c>
-      <c r="G82" t="n">
-        <v>0</v>
-      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
         <is>
-          <t>https://www.splcenter.org/fighting-hate/intelligence-report/2008/branson-televangelist-arnold-murray-preaches-christian-identity-theology</t>
+          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/ku-klux-klan</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>wetback</t>
+          <t>nazi</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2604,14 +2640,14 @@
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
         <is>
-          <t>https://www.buzzfeednews.com/article/andrewkaczynski/white-supremacists-are-thrilled-donald-trump-mentioned-opera</t>
+          <t>https://www.adl.org/resources/glossary-terms/neo-nazis</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>white genocide</t>
+          <t>neo-confederate</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2619,29 +2655,21 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
-      <c r="F84" t="n">
-        <v>22245</v>
-      </c>
-      <c r="G84" t="n">
-        <v>13</v>
-      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr">
         <is>
-          <t>https://www.adl.org/resources/glossary-terms/white-genocide</t>
+          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/neo-confederate</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>white nationalist</t>
+          <t>neo-nazi</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2649,29 +2677,21 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
-      <c r="F85" t="n">
-        <v>59520</v>
-      </c>
-      <c r="G85" t="n">
-        <v>13</v>
-      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
         <is>
-          <t>https://www.splcenter.org/fighting-hate/extremist-files/ideology/white-nationalist</t>
+          <t>https://www.adl.org/resources/glossary-terms/neo-nazis</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>white pill</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2679,29 +2699,21 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
-      <c r="F86" t="n">
-        <v>9423</v>
-      </c>
-      <c r="G86" t="n">
-        <v>10</v>
-      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr">
         <is>
-          <t>https://www.adl.org/blog/the-extremist-medicine-cabinet-a-guide-to-online-pills</t>
+          <t>https://www.washingtonpost.com/wp-srv/style/longterm/books/chap1/nigger.htm</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>white pride</t>
+          <t>stormfront</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2709,29 +2721,21 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
-      <c r="F87" t="n">
-        <v>19044</v>
-      </c>
-      <c r="G87" t="n">
-        <v>1</v>
-      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr">
         <is>
-          <t>https://www.adl.org/resources/glossary-terms/white-pride</t>
+          <t>https://www.adl.org/education/references/hate-symbols/stormfront</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>white pride worldwide</t>
+          <t>wetback</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2739,18 +2743,14 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
         <is>
-          <t>https://www.splcenter.org/fighting-hate/extremist-files/group/stormfront</t>
+          <t>https://www.buzzfeednews.com/article/andrewkaczynski/white-supremacists-are-thrilled-donald-trump-mentioned-opera</t>
         </is>
       </c>
     </row>
@@ -3808,7 +3808,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>black muslim</t>
+          <t>black power</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3818,22 +3818,22 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>566806</v>
       </c>
       <c r="G49" t="n">
-        <v>12</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>black power</t>
+          <t>electoral justice</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3849,16 +3849,16 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="n">
-        <v>566806</v>
+        <v>930</v>
       </c>
       <c r="G50" t="n">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>electoral justice</t>
+          <t>i stand with ilhan</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -3874,7 +3874,7 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="n">
-        <v>930</v>
+        <v>89</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
@@ -3883,7 +3883,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>i stand with ilhan</t>
+          <t>i stand with kaepernick</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -3899,7 +3899,7 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="n">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
@@ -3908,7 +3908,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>i stand with kaepernick</t>
+          <t>muslim american</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -3924,16 +3924,16 @@
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="n">
-        <v>25</v>
+        <v>49744</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>muslim american</t>
+          <t>muslim fashion</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -3949,16 +3949,16 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="n">
-        <v>49744</v>
+        <v>39114</v>
       </c>
       <c r="G54" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>muslim fashion</t>
+          <t>muslim parenting</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3974,16 +3974,16 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="n">
-        <v>39114</v>
+        <v>550</v>
       </c>
       <c r="G55" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>muslim parenting</t>
+          <t>muslim solidarity</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -3999,16 +3999,16 @@
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="n">
-        <v>550</v>
+        <v>733</v>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>muslim solidarity</t>
+          <t>no muslim ban ever</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4024,7 +4024,7 @@
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="n">
-        <v>733</v>
+        <v>90</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
@@ -4033,7 +4033,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>no muslim ban ever</t>
+          <t>stand with ilhan</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4049,7 +4049,7 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="n">
-        <v>90</v>
+        <v>263</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
@@ -4058,7 +4058,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>sex ed</t>
+          <t>white supremacy</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4068,18 +4068,22 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+      <c r="F59" t="n">
+        <v>309769</v>
+      </c>
+      <c r="G59" t="n">
+        <v>162</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>sex work</t>
+          <t>black muslim</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4089,18 +4093,22 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Partial Block</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>sexual liberation</t>
+          <t>sex ed</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4121,7 +4129,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>stand with ilhan</t>
+          <t>sex work</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -4131,22 +4139,18 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
-      <c r="F62" t="n">
-        <v>263</v>
-      </c>
-      <c r="G62" t="n">
-        <v>0</v>
-      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>white supremacy</t>
+          <t>sexual liberation</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -4156,17 +4160,13 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="n">
-        <v>309769</v>
-      </c>
-      <c r="G63" t="n">
-        <v>162</v>
-      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5004,7 +5004,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3d print guns</t>
+          <t>aids denial</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -5014,13 +5014,13 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -5029,7 +5029,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>abortion</t>
+          <t>ammunition clips</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -5037,16 +5037,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>678</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>aids denial</t>
+          <t>animal mating</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -5062,16 +5070,16 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>65</v>
+        <v>72001</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>alcohol</t>
+          <t>automatic gun conversion kits</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -5079,16 +5087,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>41</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ammunition</t>
+          <t>black salve</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -5096,16 +5112,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>8740</v>
+      </c>
+      <c r="G43" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ammunition clips</t>
+          <t>buy alcohol</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5121,16 +5145,16 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
-        <v>678</v>
+        <v>16087</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>animal mating</t>
+          <t>buy organs</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5146,16 +5170,16 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
-        <v>72001</v>
+        <v>43</v>
       </c>
       <c r="G45" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>automatic gun conversion kits</t>
+          <t>buy weed</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5171,16 +5195,16 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="n">
-        <v>41</v>
+        <v>26576</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>beastiality</t>
+          <t>chewing tobacco</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5188,16 +5212,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
+      <c r="F47" t="n">
+        <v>56504</v>
+      </c>
+      <c r="G47" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>beheading</t>
+          <t>execution videos</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5205,16 +5237,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
+      <c r="F48" t="n">
+        <v>3140</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>black salve</t>
+          <t>explosive vest</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5230,16 +5270,16 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
-        <v>8740</v>
+        <v>622</v>
       </c>
       <c r="G49" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>bongs</t>
+          <t>fetish content</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5247,16 +5287,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>433</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>bullfighting swords in bull</t>
+          <t>firearm scopes</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5266,22 +5314,22 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Empty</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>buy alcohol</t>
+          <t>firearm silencer</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5297,16 +5345,16 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="n">
-        <v>16087</v>
+        <v>2147</v>
       </c>
       <c r="G52" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>buy drugs on the dark web</t>
+          <t>firearm stocks</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5316,13 +5364,13 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Empty</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
@@ -5331,7 +5379,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>buy organs</t>
+          <t>generate fake credit card numbers</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -5347,16 +5395,16 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="n">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>buy weed</t>
+          <t>hunt with bombing</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -5372,16 +5420,16 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="n">
-        <v>26576</v>
+        <v>4</v>
       </c>
       <c r="G55" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>cannibus coffee shops</t>
+          <t>incorrect election date</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -5391,13 +5439,13 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Empty</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
@@ -5406,7 +5454,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>chewing tobacco</t>
+          <t>make ammunition</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -5422,16 +5470,16 @@
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="n">
-        <v>56504</v>
+        <v>476</v>
       </c>
       <c r="G57" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>cigarettes</t>
+          <t>making hard drugs</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -5439,16 +5487,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>5</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>cigars</t>
+          <t>minors drinking alcohol</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5456,16 +5512,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+      <c r="F59" t="n">
+        <v>73</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>cocaine</t>
+          <t>minors vaping</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -5473,16 +5537,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
+      <c r="F60" t="n">
+        <v>14</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>coronavirus</t>
+          <t>miracle mineral solution</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5490,16 +5562,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+      <c r="F61" t="n">
+        <v>3548</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>covid</t>
+          <t>nude photo leaks</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5507,16 +5587,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
+      <c r="F62" t="n">
+        <v>585</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>covid-19</t>
+          <t>online pharmacy no prescription</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5524,16 +5612,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>12</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>covid-19 asian food</t>
+          <t>package bombs</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5543,18 +5639,22 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>1568</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>covid-19 doesn't exist</t>
+          <t>selling firearms</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5564,18 +5664,22 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr"/>
+      <c r="F65" t="n">
+        <v>2357</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>covid-19 from 5g</t>
+          <t>terrorist acts</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5585,18 +5689,22 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
+      <c r="F66" t="n">
+        <v>11166</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>covid-19 guaranteed vaccine</t>
+          <t>terrorist attack</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5606,18 +5714,22 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr"/>
+      <c r="F67" t="n">
+        <v>485073</v>
+      </c>
+      <c r="G67" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>covid-19 home remedy</t>
+          <t>terrorist hostages</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5627,18 +5739,22 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>3</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>covid-19 people don't die</t>
+          <t>terrorist ideology</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5648,18 +5764,22 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
+      <c r="F69" t="n">
+        <v>132</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>covid-19 prayer</t>
+          <t>terrorist recruitment</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5669,18 +5789,22 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
+      <c r="F70" t="n">
+        <v>506</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>covid-19 ritual</t>
+          <t>text your vote</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5690,18 +5814,22 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
+      <c r="F71" t="n">
+        <v>287</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>covid-19 vaccine kills people</t>
+          <t>video game terrorist mod</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5711,18 +5839,22 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
+      <c r="F72" t="n">
+        <v>13</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>crystal meth</t>
+          <t>bullfighting swords in bull</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5732,18 +5864,22 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Empty</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>dog fighting</t>
+          <t>buy drugs on the dark web</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5753,22 +5889,22 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Empty</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>dramatized rape scenes</t>
+          <t>cannibus coffee shops</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -5793,7 +5929,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>e-cigarettes</t>
+          <t>dramatized rape scenes</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -5801,16 +5937,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Empty</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ecstasy</t>
+          <t>threads with firearms</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -5818,16 +5962,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Empty</t>
+        </is>
+      </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr"/>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>erotic massage services</t>
+          <t>3d print guns</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -5837,18 +5989,22 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Partial Block</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr"/>
+      <c r="F78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>escort services</t>
+          <t>dog fighting</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -5858,18 +6014,22 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Partial Block</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr"/>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr"/>
+      <c r="F79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>execution videos</t>
+          <t>make firearm</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -5879,22 +6039,22 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Partial Block</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="n">
-        <v>3140</v>
+        <v>1</v>
       </c>
       <c r="G80" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>explosive vest</t>
+          <t>make high capacity ammunition</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -5904,13 +6064,13 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Partial Block</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="n">
-        <v>622</v>
+        <v>1</v>
       </c>
       <c r="G81" t="n">
         <v>0</v>
@@ -5919,7 +6079,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>fetish content</t>
+          <t>covid-19 asian food</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -5929,22 +6089,18 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
-      <c r="F82" t="n">
-        <v>433</v>
-      </c>
-      <c r="G82" t="n">
-        <v>1</v>
-      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>firearm</t>
+          <t>covid-19 doesn't exist</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -5952,7 +6108,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr"/>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
@@ -5961,7 +6121,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>firearm scopes</t>
+          <t>covid-19 from 5g</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -5971,22 +6131,18 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
-      <c r="F84" t="n">
-        <v>3</v>
-      </c>
-      <c r="G84" t="n">
-        <v>1</v>
-      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>firearm silencer</t>
+          <t>covid-19 guaranteed vaccine</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -5996,22 +6152,18 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
-      <c r="F85" t="n">
-        <v>2147</v>
-      </c>
-      <c r="G85" t="n">
-        <v>1</v>
-      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>firearm stocks</t>
+          <t>covid-19 home remedy</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -6021,22 +6173,18 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
-      <c r="F86" t="n">
-        <v>54</v>
-      </c>
-      <c r="G86" t="n">
-        <v>0</v>
-      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>firearms</t>
+          <t>covid-19 people don't die</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -6044,7 +6192,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr"/>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
@@ -6053,7 +6205,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>covid-19 prayer</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -6061,7 +6213,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr"/>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
@@ -6070,7 +6226,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>generate fake credit card numbers</t>
+          <t>covid-19 ritual</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -6080,22 +6236,18 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr"/>
-      <c r="F89" t="n">
-        <v>99</v>
-      </c>
-      <c r="G89" t="n">
-        <v>0</v>
-      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>genitalia</t>
+          <t>covid-19 vaccine kills people</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -6103,7 +6255,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
@@ -6112,7 +6268,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>gun-grips</t>
+          <t>crystal meth</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -6120,7 +6276,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr"/>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
@@ -6129,7 +6289,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>handguns</t>
+          <t>erotic massage services</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -6137,7 +6297,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
@@ -6146,7 +6310,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>heroin</t>
+          <t>escort services</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -6154,7 +6318,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr"/>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
@@ -6163,7 +6331,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>hunt with bombing</t>
+          <t>molotov cocktail</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -6173,22 +6341,18 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
-      <c r="F94" t="n">
-        <v>4</v>
-      </c>
-      <c r="G94" t="n">
-        <v>0</v>
-      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>incest</t>
+          <t>online gambling</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -6196,7 +6360,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr"/>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
@@ -6205,7 +6373,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>incorrect election date</t>
+          <t>rolling papers</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -6215,22 +6383,18 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
-      <c r="F96" t="n">
-        <v>13</v>
-      </c>
-      <c r="G96" t="n">
-        <v>0</v>
-      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>intercourse</t>
+          <t>sex industry</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -6238,7 +6402,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr"/>
@@ -6247,7 +6415,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>make ammunition</t>
+          <t>sex services</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -6257,22 +6425,18 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
-      <c r="F98" t="n">
-        <v>476</v>
-      </c>
-      <c r="G98" t="n">
-        <v>0</v>
-      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>make firearm</t>
+          <t>sex toys</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -6282,22 +6446,18 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
-      <c r="F99" t="n">
-        <v>1</v>
-      </c>
-      <c r="G99" t="n">
-        <v>0</v>
-      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>make high capacity ammunition</t>
+          <t>sexual abuse</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -6307,22 +6467,18 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
-      <c r="F100" t="n">
-        <v>1</v>
-      </c>
-      <c r="G100" t="n">
-        <v>0</v>
-      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>making hard drugs</t>
+          <t>sexual acts</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -6332,22 +6488,18 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
-      <c r="F101" t="n">
-        <v>5</v>
-      </c>
-      <c r="G101" t="n">
-        <v>0</v>
-      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>marijuana</t>
+          <t>sexual device</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -6355,7 +6507,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr"/>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr"/>
@@ -6364,7 +6520,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>masturbation</t>
+          <t>sexual fetishes</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -6372,7 +6528,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr"/>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr"/>
@@ -6381,7 +6541,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>mephedrone</t>
+          <t>sexual fluids</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -6389,7 +6549,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr"/>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr"/>
@@ -6398,7 +6562,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>minors drinking alcohol</t>
+          <t>sexual gratification</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -6408,22 +6572,18 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
-      <c r="F105" t="n">
-        <v>73</v>
-      </c>
-      <c r="G105" t="n">
-        <v>0</v>
-      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>minors vaping</t>
+          <t>sexual harassment</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -6433,22 +6593,18 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
-      <c r="F106" t="n">
-        <v>14</v>
-      </c>
-      <c r="G106" t="n">
-        <v>0</v>
-      </c>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>miracle mineral solution</t>
+          <t>sexually explict content</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -6458,22 +6614,18 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
-      <c r="F107" t="n">
-        <v>3548</v>
-      </c>
-      <c r="G107" t="n">
-        <v>3</v>
-      </c>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>molotov cocktail</t>
+          <t>sexually unwanted acts</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -6494,7 +6646,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>nipples</t>
+          <t>vape pens</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -6502,7 +6654,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr"/>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
@@ -6511,7 +6667,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>nude photo leaks</t>
+          <t>you'll make $50,000 tomorrow with this plan!</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -6521,22 +6677,18 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
-      <c r="F110" t="n">
-        <v>585</v>
-      </c>
-      <c r="G110" t="n">
-        <v>0</v>
-      </c>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>nudity</t>
+          <t>abortion</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -6553,7 +6705,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>online gambling</t>
+          <t>alcohol</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -6561,11 +6713,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
@@ -6574,7 +6722,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>online pharmacy no prescription</t>
+          <t>ammunition</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -6582,24 +6730,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
-      <c r="F113" t="n">
-        <v>12</v>
-      </c>
-      <c r="G113" t="n">
-        <v>0</v>
-      </c>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>package bombs</t>
+          <t>beastiality</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -6607,24 +6747,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
-      <c r="F114" t="n">
-        <v>1568</v>
-      </c>
-      <c r="G114" t="n">
-        <v>0</v>
-      </c>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>pedophilia</t>
+          <t>beheading</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -6641,7 +6773,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>pornography</t>
+          <t>bongs</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -6658,7 +6790,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>prostitution</t>
+          <t>cigarettes</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -6675,7 +6807,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>rape</t>
+          <t>cigars</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -6692,7 +6824,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>rifles</t>
+          <t>cocaine</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -6709,7 +6841,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>rolling papers</t>
+          <t>coronavirus</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -6717,11 +6849,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
@@ -6730,7 +6858,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>selling firearms</t>
+          <t>covid</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -6738,24 +6866,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
-      <c r="F121" t="n">
-        <v>2357</v>
-      </c>
-      <c r="G121" t="n">
-        <v>1</v>
-      </c>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>covid-19</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -6772,7 +6892,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>sex industry</t>
+          <t>e-cigarettes</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -6780,11 +6900,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C123" t="inlineStr"/>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
@@ -6793,7 +6909,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>sex services</t>
+          <t>ecstasy</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -6801,11 +6917,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C124" t="inlineStr"/>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
@@ -6814,7 +6926,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>sex toys</t>
+          <t>firearm</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -6822,11 +6934,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C125" t="inlineStr"/>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
@@ -6835,7 +6943,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>sexual abuse</t>
+          <t>firearms</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -6843,11 +6951,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C126" t="inlineStr"/>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
@@ -6856,7 +6960,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>sexual acts</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -6864,11 +6968,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C127" t="inlineStr"/>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
@@ -6877,7 +6977,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>sexual device</t>
+          <t>genitalia</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -6885,11 +6985,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C128" t="inlineStr"/>
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
@@ -6898,7 +6994,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>sexual fetishes</t>
+          <t>gun-grips</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -6906,11 +7002,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C129" t="inlineStr"/>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
@@ -6919,7 +7011,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>sexual fluids</t>
+          <t>handguns</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -6927,11 +7019,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C130" t="inlineStr"/>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
@@ -6940,7 +7028,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>sexual gratification</t>
+          <t>heroin</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -6948,11 +7036,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C131" t="inlineStr"/>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
@@ -6961,7 +7045,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>sexual harassment</t>
+          <t>incest</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -6969,11 +7053,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C132" t="inlineStr"/>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
@@ -6982,7 +7062,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>sexually explict content</t>
+          <t>intercourse</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -6990,11 +7070,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C133" t="inlineStr"/>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
@@ -7003,7 +7079,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>sexually unwanted acts</t>
+          <t>marijuana</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -7011,11 +7087,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C134" t="inlineStr"/>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="inlineStr"/>
@@ -7024,7 +7096,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>steroids</t>
+          <t>masturbation</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -7041,7 +7113,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>suicide</t>
+          <t>mephedrone</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -7058,7 +7130,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>terrorism</t>
+          <t>nipples</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -7075,7 +7147,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>terrorist acts</t>
+          <t>nudity</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -7083,24 +7155,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C138" t="inlineStr"/>
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr"/>
-      <c r="F138" t="n">
-        <v>11166</v>
-      </c>
-      <c r="G138" t="n">
-        <v>1</v>
-      </c>
+      <c r="F138" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>terrorist attack</t>
+          <t>pedophilia</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -7108,24 +7172,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C139" t="inlineStr"/>
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr"/>
-      <c r="F139" t="n">
-        <v>485073</v>
-      </c>
-      <c r="G139" t="n">
-        <v>83</v>
-      </c>
+      <c r="F139" t="inlineStr"/>
+      <c r="G139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>terrorist hostages</t>
+          <t>pornography</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -7133,24 +7189,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C140" t="inlineStr"/>
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="inlineStr"/>
-      <c r="F140" t="n">
-        <v>3</v>
-      </c>
-      <c r="G140" t="n">
-        <v>0</v>
-      </c>
+      <c r="F140" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>terrorist ideology</t>
+          <t>prostitution</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -7158,24 +7206,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C141" t="inlineStr"/>
       <c r="D141" t="inlineStr"/>
       <c r="E141" t="inlineStr"/>
-      <c r="F141" t="n">
-        <v>132</v>
-      </c>
-      <c r="G141" t="n">
-        <v>0</v>
-      </c>
+      <c r="F141" t="inlineStr"/>
+      <c r="G141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>terrorist recruitment</t>
+          <t>rape</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -7183,24 +7223,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C142" t="inlineStr"/>
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr"/>
-      <c r="F142" t="n">
-        <v>506</v>
-      </c>
-      <c r="G142" t="n">
-        <v>0</v>
-      </c>
+      <c r="F142" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>text your vote</t>
+          <t>rifles</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -7208,24 +7240,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C143" t="inlineStr"/>
       <c r="D143" t="inlineStr"/>
       <c r="E143" t="inlineStr"/>
-      <c r="F143" t="n">
-        <v>287</v>
-      </c>
-      <c r="G143" t="n">
-        <v>0</v>
-      </c>
+      <c r="F143" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>threads with firearms</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -7233,24 +7257,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>Empty</t>
-        </is>
-      </c>
+      <c r="C144" t="inlineStr"/>
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr"/>
-      <c r="F144" t="n">
-        <v>0</v>
-      </c>
-      <c r="G144" t="n">
-        <v>0</v>
-      </c>
+      <c r="F144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>upskirt</t>
+          <t>steroids</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -7267,7 +7283,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>vape pens</t>
+          <t>suicide</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -7275,11 +7291,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C146" t="inlineStr"/>
       <c r="D146" t="inlineStr"/>
       <c r="E146" t="inlineStr"/>
       <c r="F146" t="inlineStr"/>
@@ -7288,7 +7300,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>vapes</t>
+          <t>terrorism</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -7305,7 +7317,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>vaping</t>
+          <t>upskirt</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -7322,7 +7334,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>video game terrorist mod</t>
+          <t>vapes</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -7330,24 +7342,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C149" t="inlineStr"/>
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr"/>
-      <c r="F149" t="n">
-        <v>13</v>
-      </c>
-      <c r="G149" t="n">
-        <v>0</v>
-      </c>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>voyeurism</t>
+          <t>vaping</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -7364,7 +7368,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>you'll make $50,000 tomorrow with this plan!</t>
+          <t>voyeurism</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -7372,11 +7376,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C151" t="inlineStr"/>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr"/>
       <c r="F151" t="inlineStr"/>
@@ -8133,7 +8133,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>buddhism</t>
+          <t>buddhist american</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -8141,16 +8141,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>58</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>buddhist</t>
+          <t>buddhist parenting</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -8158,16 +8166,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>16</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>buddhist american</t>
+          <t>christian american</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -8183,16 +8199,16 @@
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>58</v>
+        <v>16044</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>buddhist parenting</t>
+          <t>christian solidarity</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -8208,16 +8224,16 @@
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>16</v>
+        <v>411</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>christian american</t>
+          <t>jewish american</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -8233,16 +8249,16 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>16044</v>
+        <v>29074</v>
       </c>
       <c r="G38" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>christian solidarity</t>
+          <t>jewish parenting</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -8258,16 +8274,16 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>homosexual</t>
+          <t>jewish solidarity</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -8275,16 +8291,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>347</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>jewish american</t>
+          <t>nazi extermination camps</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -8300,16 +8324,16 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>29074</v>
+        <v>442</v>
       </c>
       <c r="G41" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>jewish parenting</t>
+          <t>nazi propoganda</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8325,7 +8349,7 @@
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>425</v>
+        <v>320</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
@@ -8334,7 +8358,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>jewish solidarity</t>
+          <t>nazi scientist</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -8350,7 +8374,7 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="n">
-        <v>347</v>
+        <v>815</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -8359,7 +8383,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>kikes</t>
+          <t>praise terrorism</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -8367,16 +8391,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
+      <c r="F44" t="n">
+        <v>3</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>muslim ttszozjqoits</t>
+          <t>praise terrorist</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -8386,13 +8418,13 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Empty</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -8401,7 +8433,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>nazi extermination camps</t>
+          <t>recruit terrorist</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -8417,7 +8449,7 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="n">
-        <v>442</v>
+        <v>29</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -8426,7 +8458,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>nazi germany</t>
+          <t>stolen election</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -8436,22 +8468,22 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Partial Block</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>11271</v>
       </c>
       <c r="G47" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>nazi propoganda</t>
+          <t>terrorism acts</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -8467,7 +8499,7 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
-        <v>320</v>
+        <v>374</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -8476,7 +8508,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>nazi scientist</t>
+          <t>terrorism attack</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -8492,16 +8524,16 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
-        <v>815</v>
+        <v>11498</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>nazis</t>
+          <t>white christian</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8509,16 +8541,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>40699</v>
+      </c>
+      <c r="G50" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>nazism</t>
+          <t>white pills</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -8526,16 +8566,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>8049</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>neo nazi</t>
+          <t>ww2 nazis</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -8545,18 +8593,22 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Blocked</t>
+          <t>Full</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
+      <c r="F52" t="n">
+        <v>849</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>neo-confederates</t>
+          <t>muslim ttszozjqoits</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -8564,16 +8616,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Empty</t>
+        </is>
+      </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>neo-nazis</t>
+          <t>nazi germany</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -8581,16 +8641,24 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Partial Block</t>
+        </is>
+      </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
+      <c r="F54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>neonazi</t>
+          <t>neo nazi</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -8598,7 +8666,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
@@ -8607,7 +8679,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>niggers</t>
+          <t>sex positive</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -8615,7 +8687,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
@@ -8624,7 +8700,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>praise terrorism</t>
+          <t>sexual education</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -8634,22 +8710,18 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Full</t>
+          <t>Blocked</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
-      <c r="F57" t="n">
-        <v>3</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0</v>
-      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>praise terrorist</t>
+          <t>buddhism</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -8657,24 +8729,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
-      <c r="F58" t="n">
-        <v>15</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0</v>
-      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>recruit terrorist</t>
+          <t>buddhist</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -8682,24 +8746,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" t="n">
-        <v>29</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0</v>
-      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>scientology</t>
+          <t>homosexual</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -8716,7 +8772,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>sex positive</t>
+          <t>kikes</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -8724,11 +8780,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
@@ -8737,7 +8789,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>sexual education</t>
+          <t>nazis</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -8745,11 +8797,7 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Blocked</t>
-        </is>
-      </c>
+      <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
@@ -8758,7 +8806,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>sexuality</t>
+          <t>nazism</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -8775,7 +8823,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>stolen election</t>
+          <t>neo-confederates</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -8783,24 +8831,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
-      <c r="F64" t="n">
-        <v>11271</v>
-      </c>
-      <c r="G64" t="n">
-        <v>16</v>
-      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>terrorism acts</t>
+          <t>neo-nazis</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -8808,24 +8848,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
-      <c r="F65" t="n">
-        <v>374</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0</v>
-      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>terrorism attack</t>
+          <t>neonazi</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -8833,24 +8865,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
-      <c r="F66" t="n">
-        <v>11498</v>
-      </c>
-      <c r="G66" t="n">
-        <v>2</v>
-      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>wetbacks</t>
+          <t>niggers</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -8867,7 +8891,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>white christian</t>
+          <t>scientology</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -8875,24 +8899,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
-      <c r="F68" t="n">
-        <v>40699</v>
-      </c>
-      <c r="G68" t="n">
-        <v>5</v>
-      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>white pills</t>
+          <t>sexuality</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -8900,24 +8916,16 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
-      <c r="F69" t="n">
-        <v>8049</v>
-      </c>
-      <c r="G69" t="n">
-        <v>2</v>
-      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ww2 nazis</t>
+          <t>wetbacks</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -8925,19 +8933,11 @@
           <t>Blocked</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Full</t>
-        </is>
-      </c>
+      <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
-      <c r="F70" t="n">
-        <v>849</v>
-      </c>
-      <c r="G70" t="n">
-        <v>0</v>
-      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>